<commit_message>
Material grafico CN 07 13 CO
Subida de material respectivo y créditos de las imagenes que lo
requieren.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/SolicitudGrafica_CN_10_02_CO_REC70.xlsx
+++ b/fuentes/contenidos/grado10/guion02/SolicitudGrafica_CN_10_02_CO_REC70.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="2360" windowWidth="35880" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -581,16 +581,7 @@
   </si>
   <si>
     <r>
-      <t>Se debe agregar una x en el eje vertical y una t en el eje horizontal a la imagen original.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
+      <t xml:space="preserve">Se debe agregar una x en el eje vertical y una t en el eje horizontal a la imagen original. Adaptadapor el autor    </t>
     </r>
     <r>
       <rPr>
@@ -1553,6 +1544,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1637,9 +1631,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -2392,8 +2383,8 @@
   <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2414,7 +2405,7 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1">
+    <row r="1" spans="1:16" ht="16" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2426,49 +2417,49 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="93"/>
+      <c r="F2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="85"/>
+      <c r="G2" s="86"/>
       <c r="H2" s="50"/>
       <c r="I2" s="50"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="93">
+      <c r="C3" s="94">
         <v>10</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="F3" s="86">
+      <c r="D3" s="95"/>
+      <c r="F3" s="87">
         <v>42065</v>
       </c>
-      <c r="G3" s="87"/>
+      <c r="G3" s="88"/>
       <c r="H3" s="50"/>
       <c r="I3" s="50"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5">
+    <row r="4" spans="1:16" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="5"/>
       <c r="F4" s="49" t="s">
         <v>55</v>
@@ -2481,15 +2472,15 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1">
+    <row r="5" spans="1:16" ht="16" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="97"/>
+      <c r="D5" s="98"/>
       <c r="E5" s="5"/>
       <c r="F5" s="47" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2503,7 +2494,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+    <row r="6" spans="1:16" ht="16" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2534,17 +2525,17 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16" thickBot="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="91"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2553,7 +2544,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="14.25" thickBot="1">
+    <row r="9" spans="1:16" ht="14" thickBot="1">
       <c r="A9" s="31" t="s">
         <v>2</v>
       </c>
@@ -2624,7 +2615,7 @@
       <c r="J10" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="K10" s="116" t="s">
+      <c r="K10" s="84" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2666,7 +2657,7 @@
       </c>
       <c r="K11" s="80"/>
     </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="15">
+    <row r="12" spans="1:16" s="12" customFormat="1">
       <c r="A12" s="76" t="s">
         <v>157</v>
       </c>
@@ -2704,7 +2695,7 @@
       </c>
       <c r="K12" s="78"/>
     </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="15">
+    <row r="13" spans="1:16" s="12" customFormat="1">
       <c r="A13" s="76" t="s">
         <v>160</v>
       </c>
@@ -2742,7 +2733,7 @@
       </c>
       <c r="K13" s="78"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="15.75">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="15">
       <c r="A14" s="76" t="s">
         <v>161</v>
       </c>
@@ -2782,7 +2773,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="15">
+    <row r="15" spans="1:16" s="12" customFormat="1">
       <c r="A15" s="76" t="s">
         <v>164</v>
       </c>
@@ -2820,7 +2811,7 @@
       </c>
       <c r="K15" s="80"/>
     </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="15">
+    <row r="16" spans="1:16" s="12" customFormat="1">
       <c r="A16" s="76" t="s">
         <v>166</v>
       </c>
@@ -2858,7 +2849,7 @@
       </c>
       <c r="K16" s="80"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="17" spans="1:11" s="12" customFormat="1">
       <c r="A17" s="76" t="s">
         <v>167</v>
       </c>
@@ -5280,38 +5271,38 @@
     <col min="12" max="16384" width="10.83203125" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
+      <c r="A1" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="102"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="103"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="104"/>
-      <c r="E2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="106"/>
       <c r="F2" s="42"/>
     </row>
-    <row r="3" spans="1:11" ht="63">
+    <row r="3" spans="1:11" ht="60">
       <c r="A3" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="41"/>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="42"/>
       <c r="H3" s="32" t="s">
         <v>18</v>
@@ -5326,7 +5317,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="40" t="s">
         <v>44</v>
       </c>
@@ -5354,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
+    <row r="5" spans="1:11" ht="76" thickBot="1">
       <c r="A5" s="43" t="s">
         <v>45</v>
       </c>
@@ -5362,11 +5353,11 @@
       <c r="C5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="112" t="str">
+      <c r="D5" s="113" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>CN_10_02_CO</v>
       </c>
-      <c r="E5" s="113"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="42"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
@@ -5381,7 +5372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1">
+    <row r="6" spans="1:11" ht="31" thickBot="1">
       <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
@@ -5403,7 +5394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
+    <row r="7" spans="1:11" ht="46" thickBot="1">
       <c r="A7" s="43" t="s">
         <v>11</v>
       </c>
@@ -5411,12 +5402,12 @@
       <c r="C7" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="98" t="str">
+      <c r="D7" s="99" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_CN_10_02_CO.xls</v>
       </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
       <c r="H7" s="32" t="s">
         <v>24</v>
       </c>
@@ -5430,7 +5421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="43" t="s">
         <v>53</v>
       </c>
@@ -5449,7 +5440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="43" t="s">
         <v>12</v>
       </c>
@@ -5468,7 +5459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1">
+    <row r="10" spans="1:11" ht="31" thickBot="1">
       <c r="A10" s="44" t="s">
         <v>36</v>
       </c>
@@ -5498,7 +5489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1">
+    <row r="12" spans="1:11" ht="16" thickBot="1">
       <c r="I12" s="32" t="s">
         <v>37</v>
       </c>
@@ -5510,14 +5501,14 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="101"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
       <c r="I13" s="32" t="s">
         <v>33</v>
       </c>
@@ -5528,7 +5519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="43"/>
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
@@ -5550,12 +5541,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="41"/>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="J15" s="32">
         <v>12</v>
       </c>
@@ -5595,12 +5586,12 @@
       <c r="C17" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="106" t="str">
+      <c r="D17" s="107" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>CN_10_02_REC10</v>
       </c>
-      <c r="E17" s="107"/>
-      <c r="F17" s="108"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="109"/>
       <c r="J17" s="32">
         <v>14</v>
       </c>
@@ -5608,7 +5599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="76" thickBot="1">
       <c r="A18" s="43" t="s">
         <v>48</v>
       </c>
@@ -5616,12 +5607,12 @@
       <c r="C18" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="98" t="str">
+      <c r="D18" s="99" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_CN_10_02_REC10.xls</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="100"/>
       <c r="J18" s="32">
         <v>15</v>
       </c>
@@ -5648,7 +5639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="61" thickBot="1">
       <c r="A20" s="44" t="s">
         <v>51</v>
       </c>
@@ -6004,7 +5995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
@@ -6026,41 +6017,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="51" t="s">
         <v>65</v>
       </c>
@@ -6183,7 +6174,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="53" customFormat="1" ht="25.5">
+    <row r="7" spans="1:11" s="53" customFormat="1" ht="28">
       <c r="A7" s="54" t="s">
         <v>80</v>
       </c>
@@ -6211,7 +6202,7 @@
       </c>
       <c r="J7" s="54"/>
     </row>
-    <row r="8" spans="1:11" s="53" customFormat="1" ht="25.5">
+    <row r="8" spans="1:11" s="53" customFormat="1" ht="28">
       <c r="A8" s="54" t="s">
         <v>82</v>
       </c>
@@ -6293,7 +6284,7 @@
       </c>
       <c r="J10" s="54"/>
     </row>
-    <row r="11" spans="1:11" s="53" customFormat="1" ht="25.5">
+    <row r="11" spans="1:11" s="53" customFormat="1" ht="28">
       <c r="A11" s="54" t="s">
         <v>89</v>
       </c>
@@ -6349,7 +6340,7 @@
       </c>
       <c r="J12" s="54"/>
     </row>
-    <row r="13" spans="1:11" ht="63">
+    <row r="13" spans="1:11" ht="60">
       <c r="A13" s="57" t="s">
         <v>93</v>
       </c>
@@ -6400,7 +6391,7 @@
       </c>
       <c r="J14" s="57"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5">
+    <row r="15" spans="1:11" ht="30">
       <c r="A15" s="57" t="s">
         <v>99</v>
       </c>
@@ -6427,7 +6418,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5">
+    <row r="16" spans="1:11" ht="90">
       <c r="A16" s="59" t="s">
         <v>103</v>
       </c>
@@ -6456,7 +6447,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5">
+    <row r="17" spans="1:11" ht="28">
       <c r="A17" s="54" t="s">
         <v>106</v>
       </c>
@@ -6529,7 +6520,7 @@
       <c r="D23" s="68"/>
       <c r="E23" s="68"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5">
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="67" t="s">
         <v>116</v>
       </c>
@@ -6555,7 +6546,7 @@
       <c r="D25" s="68"/>
       <c r="E25" s="68"/>
     </row>
-    <row r="26" spans="1:11" ht="63">
+    <row r="26" spans="1:11" ht="60">
       <c r="A26" s="67" t="s">
         <v>118</v>
       </c>

</xml_diff>